<commit_message>
Creating combined prediction data
</commit_message>
<xml_diff>
--- a/experimental_data/GEC/Keiding1988.xlsx
+++ b/experimental_data/GEC/Keiding1988.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="63">
   <si>
     <t>Keiding1988</t>
   </si>
@@ -110,6 +110,24 @@
     <t>Hepatic clearance Q*(ca-cv)/ca +- SE [ml/min]</t>
   </si>
   <si>
+    <t>Arterial concentration [mmol/L]</t>
+  </si>
+  <si>
+    <t>Arterial concentration +- SE [mmol/L]</t>
+  </si>
+  <si>
+    <t>Hepatic venous concentration [mmol/L]</t>
+  </si>
+  <si>
+    <t>Hepatic venous concentration +- SE [mmol/L]</t>
+  </si>
+  <si>
+    <t>Hepatic elimination rate Q*(ca-cv) [mmol/min]</t>
+  </si>
+  <si>
+    <t>Hepatic elimination rate Q*(ca-cv) +- SE [mmol/min]</t>
+  </si>
+  <si>
     <t>case</t>
   </si>
   <si>
@@ -125,6 +143,42 @@
     <t>infusion</t>
   </si>
   <si>
+    <t>camu</t>
+  </si>
+  <si>
+    <t>camuSE</t>
+  </si>
+  <si>
+    <t>cvmu</t>
+  </si>
+  <si>
+    <t>cvmuSE</t>
+  </si>
+  <si>
+    <t>ER</t>
+  </si>
+  <si>
+    <t>ERSE</t>
+  </si>
+  <si>
+    <t>Hemu</t>
+  </si>
+  <si>
+    <t>HemuSE</t>
+  </si>
+  <si>
+    <t>SCL</t>
+  </si>
+  <si>
+    <t>SCLSE</t>
+  </si>
+  <si>
+    <t>HCL</t>
+  </si>
+  <si>
+    <t>HCLSE</t>
+  </si>
+  <si>
     <t>ca</t>
   </si>
   <si>
@@ -137,28 +191,10 @@
     <t>cvSE</t>
   </si>
   <si>
-    <t>ER</t>
-  </si>
-  <si>
-    <t>ERSE</t>
-  </si>
-  <si>
     <t>HE</t>
   </si>
   <si>
     <t>HESE</t>
-  </si>
-  <si>
-    <t>SCL</t>
-  </si>
-  <si>
-    <t>SCLSE</t>
-  </si>
-  <si>
-    <t>HCL</t>
-  </si>
-  <si>
-    <t>HCLSE</t>
   </si>
   <si>
     <t>kei1988</t>
@@ -387,15 +423,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>99000</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>130320</xdr:rowOff>
+      <xdr:colOff>126000</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>578880</xdr:colOff>
+      <xdr:colOff>605520</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>27360</xdr:rowOff>
+      <xdr:rowOff>59040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -410,8 +446,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="99000" y="3976920"/>
-          <a:ext cx="12204360" cy="5261400"/>
+          <a:off x="126000" y="3967920"/>
+          <a:ext cx="12204000" cy="5261040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -431,10 +467,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V17"/>
+  <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T18" activeCellId="0" sqref="T18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C7" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Z11" activeCellId="0" sqref="C11:Z17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -501,7 +537,7 @@
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
     </row>
-    <row r="10" customFormat="false" ht="59.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
         <v>11</v>
       </c>
@@ -562,8 +598,26 @@
       <c r="T10" s="6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U10" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="V10" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="W10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="X10" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y10" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z10" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
         <v>11</v>
       </c>
@@ -574,66 +628,84 @@
         <v>13</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="K11" s="7" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="L11" s="7" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="M11" s="7" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="N11" s="7" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="O11" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="P11" s="7" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="Q11" s="7" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="R11" s="7" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="S11" s="7" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="T11" s="7" t="s">
-        <v>47</v>
+        <v>53</v>
+      </c>
+      <c r="U11" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V11" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="W11" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="X11" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y11" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z11" s="7" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="D12" s="8" t="n">
         <v>1</v>
@@ -686,17 +758,40 @@
       <c r="T12" s="0" t="n">
         <v>78</v>
       </c>
-      <c r="V12" s="8"/>
+      <c r="U12" s="0" t="n">
+        <f aca="false">I12/1000</f>
+        <v>0.0782</v>
+      </c>
+      <c r="V12" s="0" t="n">
+        <f aca="false">J12/1000</f>
+        <v>0.0039</v>
+      </c>
+      <c r="W12" s="0" t="n">
+        <f aca="false">K12/1000</f>
+        <v>0.0102</v>
+      </c>
+      <c r="X12" s="0" t="n">
+        <f aca="false">L12/1000</f>
+        <v>0.003</v>
+      </c>
+      <c r="Y12" s="0" t="n">
+        <f aca="false">O12/1000</f>
+        <v>0.0677</v>
+      </c>
+      <c r="Z12" s="0" t="n">
+        <f aca="false">P12/1000</f>
+        <v>0.0033</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="D13" s="8" t="n">
         <v>2</v>
@@ -749,17 +844,40 @@
       <c r="T13" s="0" t="n">
         <v>43</v>
       </c>
-      <c r="V13" s="8"/>
+      <c r="U13" s="0" t="n">
+        <f aca="false">I13/1000</f>
+        <v>0.1013</v>
+      </c>
+      <c r="V13" s="0" t="n">
+        <f aca="false">J13/1000</f>
+        <v>0.0036</v>
+      </c>
+      <c r="W13" s="0" t="n">
+        <f aca="false">K13/1000</f>
+        <v>0.0014</v>
+      </c>
+      <c r="X13" s="0" t="n">
+        <f aca="false">L13/1000</f>
+        <v>0.0024</v>
+      </c>
+      <c r="Y13" s="0" t="n">
+        <f aca="false">O13/1000</f>
+        <v>0.0843</v>
+      </c>
+      <c r="Z13" s="0" t="n">
+        <f aca="false">P13/1000</f>
+        <v>0.002</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="D14" s="8" t="n">
         <v>3</v>
@@ -812,17 +930,40 @@
       <c r="T14" s="0" t="n">
         <v>43</v>
       </c>
-      <c r="V14" s="8"/>
+      <c r="U14" s="0" t="n">
+        <f aca="false">I14/1000</f>
+        <v>0.1271</v>
+      </c>
+      <c r="V14" s="0" t="n">
+        <f aca="false">J14/1000</f>
+        <v>0.003</v>
+      </c>
+      <c r="W14" s="0" t="n">
+        <f aca="false">K14/1000</f>
+        <v>0.0189</v>
+      </c>
+      <c r="X14" s="0" t="n">
+        <f aca="false">L14/1000</f>
+        <v>0.0038</v>
+      </c>
+      <c r="Y14" s="0" t="n">
+        <f aca="false">O14/1000</f>
+        <v>0.1066</v>
+      </c>
+      <c r="Z14" s="0" t="n">
+        <f aca="false">P14/1000</f>
+        <v>0.0048</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>4</v>
@@ -875,16 +1016,40 @@
       <c r="T15" s="0" t="n">
         <v>58</v>
       </c>
+      <c r="U15" s="0" t="n">
+        <f aca="false">I15/1000</f>
+        <v>0.0775</v>
+      </c>
+      <c r="V15" s="0" t="n">
+        <f aca="false">J15/1000</f>
+        <v>0.0028</v>
+      </c>
+      <c r="W15" s="0" t="n">
+        <f aca="false">K15/1000</f>
+        <v>0.0067</v>
+      </c>
+      <c r="X15" s="0" t="n">
+        <f aca="false">L15/1000</f>
+        <v>0.0017</v>
+      </c>
+      <c r="Y15" s="0" t="n">
+        <f aca="false">O15/1000</f>
+        <v>0.0858</v>
+      </c>
+      <c r="Z15" s="0" t="n">
+        <f aca="false">P15/1000</f>
+        <v>0.0032</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>5</v>
@@ -937,16 +1102,40 @@
       <c r="T16" s="0" t="n">
         <v>69</v>
       </c>
+      <c r="U16" s="0" t="n">
+        <f aca="false">I16/1000</f>
+        <v>0.0892</v>
+      </c>
+      <c r="V16" s="0" t="n">
+        <f aca="false">J16/1000</f>
+        <v>0.0038</v>
+      </c>
+      <c r="W16" s="0" t="n">
+        <f aca="false">K16/1000</f>
+        <v>-0.0017</v>
+      </c>
+      <c r="X16" s="0" t="n">
+        <f aca="false">L16/1000</f>
+        <v>0.0028</v>
+      </c>
+      <c r="Y16" s="0" t="n">
+        <f aca="false">O16/1000</f>
+        <v>0.1106</v>
+      </c>
+      <c r="Z16" s="0" t="n">
+        <f aca="false">P16/1000</f>
+        <v>0.004</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>6</v>
@@ -998,6 +1187,30 @@
       </c>
       <c r="T17" s="0" t="n">
         <v>111</v>
+      </c>
+      <c r="U17" s="0" t="n">
+        <f aca="false">I17/1000</f>
+        <v>0.1067</v>
+      </c>
+      <c r="V17" s="0" t="n">
+        <f aca="false">J17/1000</f>
+        <v>0.0033</v>
+      </c>
+      <c r="W17" s="0" t="n">
+        <f aca="false">K17/1000</f>
+        <v>0.0163</v>
+      </c>
+      <c r="X17" s="0" t="n">
+        <f aca="false">L17/1000</f>
+        <v>0.0054</v>
+      </c>
+      <c r="Y17" s="0" t="n">
+        <f aca="false">O17/1000</f>
+        <v>0.1506</v>
+      </c>
+      <c r="Z17" s="0" t="n">
+        <f aca="false">P17/1000</f>
+        <v>0.0109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>